<commit_message>
Added logger to log particular items that seemed to not import correctly. Added in another import package for bill payments which needs to be set up.
</commit_message>
<xml_diff>
--- a/QboImporterTool/bin/Debug/items.xlsx
+++ b/QboImporterTool/bin/Debug/items.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AI Projects\QBO Customer Importer\ExcelToQBOCustomer\ExcelToQBOCustomer\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AI Projects\QBO Importer Tool\QBO Importer Tool\QboImporterTool\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Item</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>CREDIT</t>
+  </si>
+  <si>
+    <t>2:Job</t>
   </si>
 </sst>
 </file>
@@ -454,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,6 +690,26 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1.33</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Fixed up importer tool
</commit_message>
<xml_diff>
--- a/QboImporterTool/bin/Debug/items.xlsx
+++ b/QboImporterTool/bin/Debug/items.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="72">
   <si>
     <t>Item</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>Discount</t>
+  </si>
+  <si>
+    <t>2:Job</t>
   </si>
 </sst>
 </file>
@@ -649,11 +652,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K22" sqref="B22:K22"/>
+      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,17 +824,21 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
@@ -843,21 +850,17 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E8" s="2">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="2">
         <v>0</v>
       </c>
@@ -869,19 +872,21 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H9" s="2">
         <v>0</v>
       </c>
@@ -893,10 +898,10 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>54</v>
@@ -917,16 +922,16 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E11" s="2">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -941,18 +946,20 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2">
+        <v>133</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>0</v>
       </c>
       <c r="I12" s="1"/>
@@ -963,17 +970,15 @@
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
+      <c r="E13" s="2"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="3">
@@ -987,18 +992,20 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="2">
+      <c r="H14" s="3">
         <v>0</v>
       </c>
       <c r="I14" s="1"/>
@@ -1009,11 +1016,11 @@
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
@@ -1031,11 +1038,11 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
@@ -1053,11 +1060,11 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -1075,11 +1082,11 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -1097,11 +1104,11 @@
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="2">
         <v>0</v>
@@ -1119,13 +1126,11 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
@@ -1143,13 +1148,13 @@
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E21" s="2">
         <v>0</v>
@@ -1167,11 +1172,13 @@
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D22" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E22" s="2">
         <v>0</v>
@@ -1189,51 +1196,45 @@
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E23" s="2">
-        <v>1890</v>
+        <v>0</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="G23" s="1"/>
       <c r="H23" s="2">
-        <v>872</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>66</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E24" s="2">
-        <v>810</v>
+        <v>1890</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
         <v>65</v>
       </c>
       <c r="H24" s="2">
-        <v>810</v>
+        <v>872</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>66</v>
@@ -1245,40 +1246,46 @@
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="D25" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E25" s="2">
-        <v>0</v>
+        <v>810</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="H25" s="2">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1"/>
+        <v>810</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="J25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E26" s="2">
         <v>0</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
         <v>0</v>
       </c>
       <c r="I26" s="1"/>
@@ -1289,11 +1296,11 @@
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E27" s="2">
         <v>0</v>
@@ -1311,31 +1318,29 @@
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="2">
+      <c r="H28" s="3">
         <v>0</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>53</v>
@@ -1343,8 +1348,8 @@
       <c r="D29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="4">
-        <v>-1.4999999999999999E-2</v>
+      <c r="E29" s="2">
+        <v>0</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -1359,7 +1364,7 @@
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>53</v>
@@ -1368,7 +1373,7 @@
         <v>54</v>
       </c>
       <c r="E30" s="4">
-        <v>-0.08</v>
+        <v>-1.4999999999999999E-2</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1383,7 +1388,7 @@
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>53</v>
@@ -1392,7 +1397,7 @@
         <v>54</v>
       </c>
       <c r="E31" s="4">
-        <v>-0.04</v>
+        <v>-0.08</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1401,6 +1406,30 @@
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="4">
+        <v>-0.04</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>